<commit_message>
several annotation tests with no success
</commit_message>
<xml_diff>
--- a/TermRelations/data/results/patternsNVNgrouped.xlsx
+++ b/TermRelations/data/results/patternsNVNgrouped.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmchozas/Documents/GitHub/llod4lion/TermRelations/data/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A983B32-F281-C148-BAFF-DACE9725F967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B8ED3C-B113-EF40-9746-4D83A946311E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0010CFA4-505F-0942-9BE8-26585EB318C8}"/>
   </bookViews>
@@ -3154,13 +3154,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3479,7 +3479,7 @@
   <dimension ref="A1:I1497"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3494,14 +3494,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>1003</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
       <c r="G1" t="s">
         <v>1009</v>
       </c>
@@ -3522,11 +3522,11 @@
       <c r="C2" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>1001</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -3538,11 +3538,11 @@
       <c r="C3" t="s">
         <v>150</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>1007</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -3554,9 +3554,9 @@
       <c r="C4" t="s">
         <v>443</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
       <c r="G4" t="s">
         <v>1020</v>
       </c>
@@ -3574,9 +3574,9 @@
       <c r="C5" t="s">
         <v>379</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -3588,9 +3588,9 @@
       <c r="C6" t="s">
         <v>746</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
       <c r="G6" t="s">
         <v>1018</v>
       </c>
@@ -3608,9 +3608,9 @@
       <c r="C7" t="s">
         <v>150</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="G7" t="s">
         <v>1017</v>
       </c>
@@ -3625,9 +3625,9 @@
       <c r="C8" t="s">
         <v>413</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" t="s">
         <v>1013</v>
       </c>
@@ -3642,9 +3642,9 @@
       <c r="C9" t="s">
         <v>413</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
       <c r="G9" t="s">
         <v>1013</v>
       </c>
@@ -3659,11 +3659,11 @@
       <c r="C10" t="s">
         <v>255</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
       <c r="G10" t="s">
         <v>1016</v>
       </c>
@@ -3681,9 +3681,9 @@
       <c r="C11" t="s">
         <v>316</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -3695,9 +3695,9 @@
       <c r="C12" t="s">
         <v>346</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
       <c r="G12" t="s">
         <v>1014</v>
       </c>
@@ -3715,9 +3715,9 @@
       <c r="C13" t="s">
         <v>416</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -3729,9 +3729,9 @@
       <c r="C14" t="s">
         <v>487</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -3743,9 +3743,9 @@
       <c r="C15" t="s">
         <v>346</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
       <c r="G15" t="s">
         <v>1015</v>
       </c>
@@ -3760,11 +3760,11 @@
       <c r="C16" t="s">
         <v>213</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>1001</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -3776,9 +3776,9 @@
       <c r="C17" t="s">
         <v>213</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -3790,11 +3790,11 @@
       <c r="C18" t="s">
         <v>242</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>1002</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -3806,9 +3806,9 @@
       <c r="C19" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
       <c r="G19" t="s">
         <v>1023</v>
       </c>
@@ -3823,9 +3823,9 @@
       <c r="C20" t="s">
         <v>336</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
@@ -3837,9 +3837,9 @@
       <c r="C21" t="s">
         <v>231</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
       <c r="G21" t="s">
         <v>1024</v>
       </c>
@@ -3854,9 +3854,9 @@
       <c r="C22" t="s">
         <v>504</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
@@ -3868,9 +3868,9 @@
       <c r="C23" t="s">
         <v>242</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -3882,9 +3882,9 @@
       <c r="C24" t="s">
         <v>604</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -3896,9 +3896,9 @@
       <c r="C25" t="s">
         <v>574</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
@@ -3910,9 +3910,9 @@
       <c r="C26" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
@@ -3924,9 +3924,9 @@
       <c r="C27" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
@@ -3938,9 +3938,9 @@
       <c r="C28" t="s">
         <v>946</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
@@ -3952,9 +3952,9 @@
       <c r="C29" t="s">
         <v>273</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -3966,11 +3966,11 @@
       <c r="C30" t="s">
         <v>831</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="4" t="s">
         <v>1001</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
@@ -3982,9 +3982,9 @@
       <c r="C31" t="s">
         <v>221</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
@@ -3996,9 +3996,9 @@
       <c r="C32" t="s">
         <v>225</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
@@ -4010,9 +4010,9 @@
       <c r="C33" t="s">
         <v>300</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
@@ -4024,11 +4024,11 @@
       <c r="C34" t="s">
         <v>98</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="5" t="s">
         <v>1004</v>
       </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -4040,9 +4040,9 @@
       <c r="C35" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
@@ -4054,9 +4054,9 @@
       <c r="C36" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
@@ -4068,9 +4068,9 @@
       <c r="C37" t="s">
         <v>340</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
@@ -4082,9 +4082,9 @@
       <c r="C38" t="s">
         <v>135</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
@@ -4096,9 +4096,9 @@
       <c r="C39" t="s">
         <v>300</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
@@ -4110,9 +4110,9 @@
       <c r="C40" t="s">
         <v>782</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
@@ -4124,9 +4124,9 @@
       <c r="C41" t="s">
         <v>847</v>
       </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
@@ -4138,9 +4138,9 @@
       <c r="C42" t="s">
         <v>268</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
@@ -4152,9 +4152,9 @@
       <c r="C43" t="s">
         <v>701</v>
       </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
@@ -4166,9 +4166,9 @@
       <c r="C44" t="s">
         <v>701</v>
       </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
@@ -4180,11 +4180,11 @@
       <c r="C45" t="s">
         <v>300</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="4" t="s">
         <v>1005</v>
       </c>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
@@ -4196,9 +4196,9 @@
       <c r="C46" t="s">
         <v>300</v>
       </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
@@ -4210,9 +4210,9 @@
       <c r="C47" t="s">
         <v>300</v>
       </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
@@ -4224,9 +4224,9 @@
       <c r="C48" t="s">
         <v>300</v>
       </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
@@ -4238,9 +4238,9 @@
       <c r="C49" t="s">
         <v>300</v>
       </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
@@ -4252,9 +4252,9 @@
       <c r="C50" t="s">
         <v>648</v>
       </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
@@ -4266,9 +4266,9 @@
       <c r="C51" t="s">
         <v>300</v>
       </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
@@ -4280,11 +4280,11 @@
       <c r="C52" t="s">
         <v>134</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="5" t="s">
         <v>1008</v>
       </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
@@ -4296,9 +4296,9 @@
       <c r="C53" t="s">
         <v>189</v>
       </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
@@ -4310,9 +4310,9 @@
       <c r="C54" t="s">
         <v>411</v>
       </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
@@ -4324,9 +4324,9 @@
       <c r="C55" t="s">
         <v>574</v>
       </c>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
@@ -4338,9 +4338,9 @@
       <c r="C56" t="s">
         <v>300</v>
       </c>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
@@ -4352,9 +4352,9 @@
       <c r="C57" t="s">
         <v>300</v>
       </c>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
@@ -4366,9 +4366,9 @@
       <c r="C58" t="s">
         <v>67</v>
       </c>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
@@ -4380,9 +4380,9 @@
       <c r="C59" t="s">
         <v>57</v>
       </c>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
@@ -4394,9 +4394,9 @@
       <c r="C60" t="s">
         <v>649</v>
       </c>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
@@ -4408,9 +4408,9 @@
       <c r="C61" t="s">
         <v>649</v>
       </c>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
@@ -4422,9 +4422,9 @@
       <c r="C62" t="s">
         <v>221</v>
       </c>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
@@ -4436,9 +4436,9 @@
       <c r="C63" t="s">
         <v>67</v>
       </c>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
@@ -4450,9 +4450,9 @@
       <c r="C64" t="s">
         <v>574</v>
       </c>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
@@ -4464,9 +4464,9 @@
       <c r="C65" t="s">
         <v>574</v>
       </c>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
@@ -4478,9 +4478,9 @@
       <c r="C66" t="s">
         <v>221</v>
       </c>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
@@ -4492,9 +4492,9 @@
       <c r="C67" t="s">
         <v>150</v>
       </c>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
@@ -4506,9 +4506,9 @@
       <c r="C68" t="s">
         <v>789</v>
       </c>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
@@ -4520,9 +4520,9 @@
       <c r="C69" t="s">
         <v>884</v>
       </c>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
@@ -4534,9 +4534,9 @@
       <c r="C70" t="s">
         <v>900</v>
       </c>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
@@ -4548,9 +4548,9 @@
       <c r="C71" t="s">
         <v>900</v>
       </c>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
@@ -4562,9 +4562,9 @@
       <c r="C72" t="s">
         <v>906</v>
       </c>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
@@ -4576,9 +4576,9 @@
       <c r="C73" t="s">
         <v>57</v>
       </c>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
@@ -4590,9 +4590,9 @@
       <c r="C74" t="s">
         <v>57</v>
       </c>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
@@ -4604,9 +4604,9 @@
       <c r="C75" t="s">
         <v>300</v>
       </c>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
@@ -4618,9 +4618,9 @@
       <c r="C76" t="s">
         <v>934</v>
       </c>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
@@ -4632,9 +4632,9 @@
       <c r="C77" t="s">
         <v>963</v>
       </c>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
@@ -4646,9 +4646,9 @@
       <c r="C78" t="s">
         <v>57</v>
       </c>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
@@ -4660,9 +4660,9 @@
       <c r="C79" t="s">
         <v>986</v>
       </c>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
@@ -4674,9 +4674,9 @@
       <c r="C80" t="s">
         <v>187</v>
       </c>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
@@ -4688,9 +4688,9 @@
       <c r="C81" t="s">
         <v>187</v>
       </c>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
@@ -4702,9 +4702,9 @@
       <c r="C82" t="s">
         <v>213</v>
       </c>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
@@ -4716,9 +4716,9 @@
       <c r="C83" t="s">
         <v>213</v>
       </c>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
@@ -4730,9 +4730,9 @@
       <c r="C84" t="s">
         <v>421</v>
       </c>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
@@ -4744,9 +4744,9 @@
       <c r="C85" t="s">
         <v>421</v>
       </c>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
@@ -4758,9 +4758,9 @@
       <c r="C86" t="s">
         <v>187</v>
       </c>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
@@ -4772,9 +4772,9 @@
       <c r="C87" t="s">
         <v>187</v>
       </c>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
@@ -20291,17 +20291,17 @@
     <sortCondition ref="B2:B1497"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="D80:F87"/>
+    <mergeCell ref="D18:F29"/>
+    <mergeCell ref="D30:F33"/>
+    <mergeCell ref="D34:F44"/>
+    <mergeCell ref="D45:F51"/>
+    <mergeCell ref="D52:F79"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="D3:F9"/>
     <mergeCell ref="D10:F15"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="D16:F17"/>
-    <mergeCell ref="D18:F29"/>
-    <mergeCell ref="D30:F33"/>
-    <mergeCell ref="D34:F44"/>
-    <mergeCell ref="D45:F51"/>
-    <mergeCell ref="D52:F79"/>
-    <mergeCell ref="D80:F87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>